<commit_message>
Acabado para un 8, vamos a por el 10
</commit_message>
<xml_diff>
--- a/M10_Sistemas_Gestión_Empresas/UF1/P6/odooIkeaChairs.xlsx
+++ b/M10_Sistemas_Gestión_Empresas/UF1/P6/odooIkeaChairs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IES_Marianao\DAM\Segundo\M10_Sistemas_Gestión_Empresas\UF1\P6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IES_Marianao\DAM\Segundo\M10_Sistemas_Gestión_Empresas\UF1\P6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213645C1-4BE7-4A0F-AACE-B2C7EB2E654A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B55804-C1E2-44B8-83CF-04D6681A1E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -69,10 +69,13 @@
     <t>All / Saleable / Office Furniture</t>
   </si>
   <si>
-    <t>White</t>
-  </si>
-  <si>
     <t>Product Attributes/Values</t>
+  </si>
+  <si>
+    <t>White,Yellow</t>
+  </si>
+  <si>
+    <t>Aluminium,Steel</t>
   </si>
 </sst>
 </file>
@@ -394,7 +397,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,7 +436,7 @@
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I1" t="s">
         <v>7</v>
@@ -462,7 +465,7 @@
         <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -472,8 +475,8 @@
       <c r="G3" t="s">
         <v>12</v>
       </c>
-      <c r="H3">
-        <v>4</v>
+      <c r="H3" t="s">
+        <v>16</v>
       </c>
       <c r="I3" s="1"/>
     </row>

</xml_diff>